<commit_message>
debugging akurasi, labeling, dan visualisasi
</commit_message>
<xml_diff>
--- a/public/file_dataset/testing firstmedia 2020-12-01.xlsx
+++ b/public/file_dataset/testing firstmedia 2020-12-01.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="53">
   <si>
     <t>id_tweet</t>
   </si>
@@ -37,143 +37,133 @@
     <t>FirstMediaCares</t>
   </si>
   <si>
-    <t>brendyyi</t>
+    <t>alphavityazi</t>
   </si>
   <si>
     <t>fuckinghard6969</t>
   </si>
   <si>
-    <t>Geraldy_Gteam</t>
-  </si>
-  <si>
-    <t>lythix_</t>
-  </si>
-  <si>
-    <t>saferaaa</t>
-  </si>
-  <si>
-    <t>blckrd25</t>
-  </si>
-  <si>
     <t>rezapati</t>
   </si>
   <si>
-    <t>@Bezallael_Antok Hi First People. Mohon maaf atas ketidaknyamanannya. Saat ini teknisi jaringan kami sedang melakukan proses perbaikan agar problem tersebut dapat segera normal. Untuk problem ini silahkan Bpk/Ibu mengakses di situs https://t.co/h46Z2K7k7Z. Tks ^myo</t>
+    <t>notapetite</t>
+  </si>
+  <si>
+    <t>@bruntus182 Selamat Malam First People. Mhn maaf sebelumnya Jika kami cek untuk area Ibu/Bapak terpantau sdh normal, mohon info saat ini kendala pd layanan Internet atau TV ya? mengenai jaringan dan tagihan Bapak / Ibu bisa mengaksesnya di situs https://t.co/h46Z2K7k7Z . Tks ^dhp</t>
+  </si>
+  <si>
+    <t>@Ferry14939796 Hi First People, baik Pak kami akan upayakan utk perbaikannya mohon kesediaannya menunggu progres team terkait utk info selanjutnya bisa cek https://t.co/JMlireD1it terima kasih. ^rml</t>
   </si>
   <si>
     <t>@RsDayshe Selamat Malam First People, mohon maaf atas ketidaknyamanannya ya atas gangguan jaringan on-off saat ini mohon kesediaannya menunggu progres team terkait ya utk info lebih lanjut cek https://t.co/JMlireD1it terima kasih. ^rml</t>
   </si>
   <si>
-    <t>@FirstMediaCares Cape bro komplain, liat akun saya ini tweet cuman komplain ke firstmedia doang paling sering,</t>
-  </si>
-  <si>
-    <t>@pemfitraan @FirstMediaCares Nyesel kan pake firstmedia sama saya juga</t>
-  </si>
-  <si>
-    <t>@FirstMediaCares no pelanggan saya ya  47686401 , gak bisa dm soalnya ke firstmedia nihh</t>
-  </si>
-  <si>
-    <t>@su3sno Selamat Malam First People, mohon maaf saat ini gangguan area dan masih dlm upaya perbaikan gangguan jaringan area. Waktu perbaikan 02-Dec-2020 / 01:53 mohon kesediaannya menunggu utk info selanjutnya bisa cek https://t.co/JMlireD1it terima kasih ^rml</t>
-  </si>
-  <si>
-    <t>@evilmorty07 
-Hi FIRST people. Mohon ditunggu prosesnnya , diusahakan perbaikan seoptimal mungkin untuk perbaikan agar sesegera mungkin areanya normal kembali . utk informasi terakhir mengenai problem ini silakan akses di https://t.co/h46Z2K7k7Z. Tks. ^Fuj</t>
-  </si>
-  <si>
-    <t>@adiaries Selamat Malam First Poeple. Mohon maaf atas ketidaknyamanannya. Saat ini sdg ada gangguan jaringan di area Bapak/Ibu dan msh dlm proses perbaikan oleh tim terkait kami. Untuk updatenya bisa akses https://t.co/h46Z2K7k7Z. Tks ^RZA</t>
-  </si>
-  <si>
-    <t>apasi anj firstmedia idup mati idup mati ngerjain quizziz aj ribet terus lagi main genshin gk lancar 😤😤</t>
-  </si>
-  <si>
-    <t>@iesheanandr Selamat Malam First Poeple. Mohon maaf atas ketidaknyamanannya. Saat ini sdg ada gangguan jaringan di area Bapak/Ibu dan msh dlm proses perbaikan oleh tim terkait kami. Untuk updatenya bisa akses https://t.co/h46Z2K7k7Z. Tks ^RZA</t>
-  </si>
-  <si>
-    <t>@calondudawakaka Selamat Siang First Poeple. Mohon maaf atas ketidaknyamanannya. Saat ini sdg ada gangguan jaringan di area Bapak/Ibu dan msh dlm proses perbaikan oleh tim terkait kami. Untuk updatenya bisa akses https://t.co/h46Z2K7k7Z. Tks ^RZA</t>
-  </si>
-  <si>
-    <t>@Aoyama17Kei Hi First People. Mhn maaf atas ktdknyamanannya. Memaksimalkan perbaikn gangguan layanan tsb. Untuk informasi terakhir mengenai masalah ini dapat mengaksesnya melalui https://t.co/h46Z2K7k7Z. Tks ^mrs</t>
-  </si>
-  <si>
-    <t>@habepeh Selamat siang First People. Mohon maaf atas ketidaknyamanannya. Saat ini sdg terjadi prblm jaringan signal quality. Mohon kesediannya menunggu hingga 3 hari kedepan utk perbaikannya. Detailnya bisa lihat di https://t.co/h46Z2K7k7Z. Tks ^Gio</t>
-  </si>
-  <si>
-    <t>@janganordinary  Hi First People , mohon maaf atas kendala sebelumnya, semoga kendala cepat teratasi ya dan selamat beraktifitas kembali. Info jaringan dan tagihan  bisa pantau di https://t.co/h46Z2K7k7Z atau myFirstMedia App. Tks ^em</t>
-  </si>
-  <si>
-    <t>@giphuuu Hi First People. Mohon maaf atas ketidaknyamanannya. Saat ini akunnya sedang terblokir. Mohon lakukan pembayarannya dahulu ya agar dapat kami buka blokirannya. Untuk informasi billing dan lainnya bisa lihat di https://t.co/h46Z2K7k7Z. Tks ^Gio</t>
-  </si>
-  <si>
-    <t>@eeyorejunior  Selamat Pagi First People. Mohon maaf . Saat ini sdg terjadi prblm jaringan dan sdg dalam perbaikan.  Estimasi waktu perbaikan 02-Dec-2020 / 10:46. Info jaringan dan tagihan bisa pantau di https://t.co/h46Z2K7k7Z atau myFirstMedia App. Tks ^em</t>
-  </si>
-  <si>
-    <t>@FirstMediaCares Saya gatau ini udah keluhan keberapa kalinya. Internet dirumah saya sering sekali putus nyambung, saya minta datangkan teknisi tapi dari firstmedia cuma bilang maaf. Adik adik saya jadinya tidak bisa mengikuti pelajaran karena jeleknya jaringan dari firstmedia</t>
-  </si>
-  <si>
-    <t>@FirstMediaCares siang, untuk nopel 11127925 di cek firstmedia keterangannya online tapi kok di modem indikator onlinenya mati ya. Bisa dibantu cek? Terima kasih</t>
+    <t>@godjila526 Selamat malam first people,mhn maaf atas ketidaknyamanan.Saat ini area anda mengalami gangguan quality signal sehingga internet slow, on off bahkan offline dan saat ini masih dalam proses perbaikan oleh tim terkait.Detailnya https://t.co/h46Z2K7k7Z.Tks ^Fjr</t>
+  </si>
+  <si>
+    <t>@nina_mayoni Selamat malam first people,mhn maaf atas ketidaknyamanan.Saat ini area anda mengalami gangguan quality signal sehingga internet on off bahkan offline dan saat ini masih dalam proses perbaikan oleh tim terkait.Detailnya https://t.co/h46Z2K7k7Z.Tks ^Fjr</t>
+  </si>
+  <si>
+    <t>@FirstMediaCares setelah dicek, lalu apa? ini udah sekitar 2-3 hari gangguan di website cek firstmedia, tp ga ada perubahan. gausah perubahan, estimasi perbaikan aja gak jelas s/d kapan. belum lagi rto rto yang terjadi sudah hampir 2 minggu lebih.</t>
+  </si>
+  <si>
+    <t>@redblueexh Hi first people, mohon maaf atas ketidaknyamanannya perihal gangguan jaringan di area rmh Bapak/Ibu saat ini dan msh dalam proses perbaikan. Update infonya ada di https://t.co/h46Z2K7k7Z ya. Tks ^tst</t>
+  </si>
+  <si>
+    <t>@OgawaRen Selamat malam First People, mohon maaf atas ketidaknyamanannya. Saat ini area Bpk/Ibu sdg mengalami gangguan jaringan. Namun akan kami upayakan secepatnya. Informasi mengenai status area tsb silahkan dicek di https://t.co/IQIwB9XHrI. Terimakasih ^ang</t>
+  </si>
+  <si>
+    <t>@febriani_p @FirstMediaCares Emang aneh2 aja first media skrg.. boikot aja firstmedia</t>
+  </si>
+  <si>
+    <t>@davfadel Selamat Malam First People. Mohon maaf saat ini sdg terjadi prblm jaringan dan hal ini sdh dalam proses perbaikan dari team jaringan kami. Estimasi waktu perbaikan 02-Dec-2020 / 07:58. Detailnya bisa pantau di https://t.co/h46Z2K7k7Z. Tks ^Ibn</t>
+  </si>
+  <si>
+    <t>@Aldry_F Selamat malam First People. Mhn maaf atas ketidaknyamanannya. Kami cek area saat ini normal, mhn restart kabel pwr modem ya. Jika masih kendala mhn dicoba utk bypass dr modem lgsg dgn kabel LAN ya. Untuk cek &amp;amp; refresh jaringan bs di https://t.co/h46Z2K7k7Z ya. Tks. ^Fjr</t>
+  </si>
+  <si>
+    <t>@sen9922 Selamat malam FIRST people. Mohon maaf atas ketidaknyamanan yang dialami. Saat ini areanya masih dalam prses perbaikan, yang menyebabkan kualitas jaringan areannya  menurun.  untuk cek status perbaikan bisa cek di https://t.co/h46Z2K7k7Z . Tks ^Fuj</t>
+  </si>
+  <si>
+    <t>@rizkybayumilano   Selamat Siang First People. Mohon maaf atas ketidaknyamanannya. Saat ini sdg terjadi prblm jaringan signal quality. Detail jaringan dan tagihan bisa pantau di https://t.co/h46Z2K7k7Z  dan MYFirstMedia App ^em</t>
+  </si>
+  <si>
+    <t>@rahmat_sitinjak Slmt Siang First People. Mhn maaf atas ktdknyamanannya. Sdg terjadi gangguan layanan area ASEM BARIS, adapun perkiraan estimasi perbaikan sampai dgn 01-Dec-2020 / 21:18. Utk info terakhir mengenai mslh ini dpt mengaksesnya via https://t.co/h46Z2K7k7Z. Tks ^mrs</t>
+  </si>
+  <si>
+    <t>@soreschach Selamat Siang First Poeple. Mohon maaf atas ketidaknyamanannya. Saat ini sdg ada gangguan jaringan di area Bapak/Ibu dan msh dlm proses perbaikan oleh tim terkait kami. Untuk updatenya bisa akses https://t.co/h46Z2K7k7Z. Tks ^RZA</t>
+  </si>
+  <si>
+    <t>@boreg8401 Hi First People. Mhn maaf atas kendalanya dan terima kasih inputannya untuk perbaikan layanan kami. Untuk update info status jaringan kami sarankan untuk cek di https://t.co/h46Z2K7k7Z ya. Tks ^mel</t>
+  </si>
+  <si>
+    <t>@kabigon89    Selamat  pagi  First People. Mohon maaf atas ketidaknyamanannya. Saat ini sdg terjadi gangguan jaringan. estimasi waktu 01-Dec-2020 / 22:52 kami sedang upayakan segera normal,  Detailnya bisa pantau di https://t.co/h46Z2K7k7Z. Tks ^Sth</t>
   </si>
   <si>
     <t>@FirstMediaCares parah nih firstmedia dalam seminggu 2x gangguan. Perusahaan besar dan lama tapi belum bisa meminimalisir gangguan. Ditambah disaat orang sedang butuh koneksi internet. Mmm.. sudah waktunya cari-cari alternatif lain nih.</t>
   </si>
   <si>
+    <t>firstmedia masi pagi udh gajelas☺️🙏🏻</t>
+  </si>
+  <si>
     <t>@HafidRehaff Selamat Pagi First People, mohon maaf atas ketidaknyamanannya. Kami informasikan untuk saat ini area sedang mengalami gangguan, estimasi waktu perbaikan diperkirakan 02-Dec-2020 / 01:26. Info status jaringan dpt akses di https://t.co/h46Z2K7k7Z. Terima kasih ^nlv</t>
   </si>
   <si>
-    <t>2020-12-01 15:57:56</t>
+    <t>2020-12-01 15:34:45</t>
+  </si>
+  <si>
+    <t>2020-12-01 15:27:05</t>
   </si>
   <si>
     <t>2020-12-01 15:24:36</t>
   </si>
   <si>
-    <t>2020-12-01 15:22:32</t>
-  </si>
-  <si>
-    <t>2020-12-01 13:12:31</t>
-  </si>
-  <si>
-    <t>2020-12-01 13:03:25</t>
-  </si>
-  <si>
-    <t>2020-12-01 12:49:30</t>
-  </si>
-  <si>
-    <t>2020-12-01 12:45:58</t>
-  </si>
-  <si>
-    <t>2020-12-01 12:42:39</t>
-  </si>
-  <si>
-    <t>2020-12-01 12:25:57</t>
-  </si>
-  <si>
-    <t>2020-12-01 12:09:27</t>
-  </si>
-  <si>
-    <t>2020-12-01 06:38:59</t>
-  </si>
-  <si>
-    <t>2020-12-01 06:37:19</t>
-  </si>
-  <si>
-    <t>2020-12-01 06:36:23</t>
-  </si>
-  <si>
-    <t>2020-12-01 04:58:58</t>
-  </si>
-  <si>
-    <t>2020-12-01 04:54:08</t>
-  </si>
-  <si>
-    <t>2020-12-01 04:45:24</t>
-  </si>
-  <si>
-    <t>2020-12-01 04:22:20</t>
-  </si>
-  <si>
-    <t>2020-12-01 04:10:23</t>
+    <t>2020-12-01 15:08:25</t>
+  </si>
+  <si>
+    <t>2020-12-01 14:56:52</t>
+  </si>
+  <si>
+    <t>2020-12-01 14:36:51</t>
+  </si>
+  <si>
+    <t>2020-12-01 13:47:37</t>
+  </si>
+  <si>
+    <t>2020-12-01 13:37:18</t>
+  </si>
+  <si>
+    <t>2020-12-01 13:12:05</t>
+  </si>
+  <si>
+    <t>2020-12-01 13:03:40</t>
+  </si>
+  <si>
+    <t>2020-12-01 11:51:08</t>
+  </si>
+  <si>
+    <t>2020-12-01 11:47:25</t>
+  </si>
+  <si>
+    <t>2020-12-01 07:22:01</t>
+  </si>
+  <si>
+    <t>2020-12-01 06:09:10</t>
+  </si>
+  <si>
+    <t>2020-12-01 05:51:06</t>
+  </si>
+  <si>
+    <t>2020-12-01 05:30:06</t>
+  </si>
+  <si>
+    <t>2020-12-01 04:10:36</t>
   </si>
   <si>
     <t>2020-12-01 03:32:10</t>
+  </si>
+  <si>
+    <t>2020-12-01 01:55:45</t>
   </si>
   <si>
     <t>2020-12-01 01:54:51</t>
@@ -568,382 +558,382 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>1.33380251970159E+18</v>
+        <v>1.333796685911233E+18</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>1.333794130921615E+18</v>
+        <v>1.333794758850843E+18</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>1.333793614229504E+18</v>
+        <v>1.333794130921615E+18</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>1.333760894543618E+18</v>
+        <v>1.333790058327855E+18</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>1.33375860163933E+18</v>
+        <v>1.333787153592058E+18</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>1.333755100804698E+18</v>
+        <v>1.333782113636684E+18</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>1.333754210605679E+18</v>
+        <v>1.333769726556705E+18</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>1.333753375641403E+18</v>
+        <v>1.333767129007493E+18</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>1.333749174630695E+18</v>
+        <v>1.333760783608529E+18</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>1.33374502101982E+18</v>
+        <v>1.333758666256708E+18</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>1.33366185640208E+18</v>
+        <v>1.333740413656527E+18</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <v>1.333661438854894E+18</v>
+        <v>1.33373947439247E+18</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <v>1.333661202648429E+18</v>
+        <v>1.333672686745121E+18</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
-        <v>1.333636685746172E+18</v>
+        <v>1.333654353995973E+18</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
-        <v>1.333635470534742E+18</v>
+        <v>1.333649804295959E+18</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17">
-        <v>1.333633273788989E+18</v>
+        <v>1.333644522337694E+18</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18">
-        <v>1.333627466980618E+18</v>
+        <v>1.333624515889222E+18</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19">
-        <v>1.333624462026019E+18</v>
+        <v>1.333614841504797E+18</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20">
-        <v>1.333614841504797E+18</v>
+        <v>1.333590577875624E+18</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -954,16 +944,16 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>